<commit_message>
added Data Driven features
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/Data.xlsx
+++ b/src/main/resources/testData/Data.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="14700" tabRatio="835" activeTab="2"/>
+    <workbookView windowHeight="16940" tabRatio="835" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="28" r:id="rId1"/>
     <sheet name="13.Shortcut" sheetId="38" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="48" r:id="rId3"/>
+    <sheet name="orders" sheetId="48" r:id="rId3"/>
+    <sheet name="openMRS" sheetId="49" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ExtraCredit">#REF!</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="196">
   <si>
     <t xml:space="preserve">
 </t>
@@ -347,10 +348,10 @@
     <t>Product</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>CustomerName</t>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
   <si>
     <t>Street</t>
@@ -368,10 +369,13 @@
     <t>Card</t>
   </si>
   <si>
-    <t>CardNumber</t>
-  </si>
-  <si>
-    <t>ExpireDate</t>
+    <t>Card Number</t>
+  </si>
+  <si>
+    <t>Exp</t>
+  </si>
+  <si>
+    <t>SuccessMessage</t>
   </si>
   <si>
     <t>MyMoney</t>
@@ -395,6 +399,12 @@
     <t>1298764514397150</t>
   </si>
   <si>
+    <t>09/27</t>
+  </si>
+  <si>
+    <t>New order has been successfully added.</t>
+  </si>
+  <si>
     <t>FamilyAlbum</t>
   </si>
   <si>
@@ -471,22 +481,162 @@
   </si>
   <si>
     <t>143 Main st</t>
+  </si>
+  <si>
+    <t>Given</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Family Name</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Address 2</t>
+  </si>
+  <si>
+    <t>City/Village</t>
+  </si>
+  <si>
+    <t>State/Province</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Du</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>123 Main St</t>
+  </si>
+  <si>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Jhonson</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>124 Main St</t>
+  </si>
+  <si>
+    <t>Brentwood</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Len</t>
+  </si>
+  <si>
+    <t>Davidson</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>125 Main St</t>
+  </si>
+  <si>
+    <t>Spring Hill</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>126 Main St</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>127 Main St</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>128 Main St</t>
+  </si>
+  <si>
+    <t>September</t>
+  </si>
+  <si>
+    <t>129 Main St</t>
+  </si>
+  <si>
+    <t>October</t>
+  </si>
+  <si>
+    <t>130 Main St</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>131 Main St</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
-    <numFmt numFmtId="176" formatCode="mm/yy"/>
+  <numFmts count="8">
+    <numFmt numFmtId="176" formatCode="&quot;Highlight&quot;;&quot;&quot;;&quot;&quot;"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="\¥#,##0_);\(\¥#,##0\)"/>
+    <numFmt numFmtId="179" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="177" formatCode="\¥#,##0_);\(\¥#,##0\)"/>
-    <numFmt numFmtId="178" formatCode="yyyy;@"/>
-    <numFmt numFmtId="179" formatCode="yyyy&quot;年&quot;m&quot;月&quot;d&quot;日&quot;;@"/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="181" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="182" formatCode="&quot;Highlight&quot;;&quot;&quot;;&quot;&quot;"/>
-    <numFmt numFmtId="183" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="182" formatCode="yyyy;@"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -560,14 +710,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -583,15 +725,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -610,6 +746,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -617,11 +768,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.349986266670736"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -640,32 +797,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei UI"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.349986266670736"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -676,25 +819,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Microsoft YaHei UI"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -719,19 +869,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF217346"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -743,7 +881,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -755,31 +893,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.0499893185216834"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -797,13 +941,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -815,19 +1049,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -839,85 +1061,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.0499893185216834"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -946,77 +1096,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF339966"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF339966"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF339966"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color rgb="FF339966"/>
@@ -1039,26 +1122,96 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF339966"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF339966"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF339966"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FFF4B183"/>
-      </left>
-      <right style="thick">
-        <color rgb="FFF4B183"/>
-      </right>
-      <top style="thick">
-        <color rgb="FFF4B183"/>
-      </top>
-      <bottom style="thick">
-        <color rgb="FFF4B183"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1085,26 +1238,23 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color rgb="FF339966"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
+      <left style="thick">
+        <color rgb="FFF4B183"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
+      <right style="thick">
+        <color rgb="FFF4B183"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFF4B183"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFF4B183"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1112,158 +1262,158 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="182" fontId="29" fillId="0" borderId="0" applyFill="0" applyBorder="0">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyFill="0" applyBorder="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="176" fontId="27" fillId="0" borderId="0" applyFill="0" applyBorder="0">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="15"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="20" fillId="0" borderId="0">
+      <alignment horizontal="right" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10"/>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="25" fillId="0" borderId="0">
-      <alignment horizontal="right" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="6" fontId="0" fillId="29" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="6" fontId="0" fillId="18" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="4"/>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyNumberFormat="0" applyFont="0" applyFill="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="17" fillId="7" borderId="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyNumberFormat="0" applyFont="0" applyFill="0"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="15" fillId="5" borderId="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="183" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="181" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="left" wrapText="1" indent="4"/>
     </xf>
-    <xf numFmtId="180" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="181" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1274,7 +1424,7 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1300,7 +1450,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="65" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -1318,12 +1468,12 @@
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Highlight Icon" xfId="1"/>
-    <cellStyle name="绿色左边框" xfId="2"/>
-    <cellStyle name="开始文本" xfId="3"/>
-    <cellStyle name="下边框" xfId="4"/>
-    <cellStyle name="左边框" xfId="5"/>
-    <cellStyle name="绿色右边框" xfId="6"/>
+    <cellStyle name="绿色右边框" xfId="1"/>
+    <cellStyle name="左边框" xfId="2"/>
+    <cellStyle name="下边框" xfId="3"/>
+    <cellStyle name="开始文本" xfId="4"/>
+    <cellStyle name="绿色左边框" xfId="5"/>
+    <cellStyle name="Highlight Icon" xfId="6"/>
     <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
     <cellStyle name="40% - Accent6" xfId="8" builtinId="51"/>
     <cellStyle name="橙色边框" xfId="9"/>
@@ -2384,10 +2534,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView zoomScale="128" zoomScaleNormal="128" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.94117647058824" defaultRowHeight="16.8"/>
@@ -2402,9 +2552,10 @@
     <col min="8" max="8" width="15.6470588235294" customWidth="1"/>
     <col min="9" max="9" width="16.7647058823529" customWidth="1"/>
     <col min="10" max="10" width="9.82352941176471" customWidth="1"/>
+    <col min="11" max="11" width="34.5294117647059" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -2435,677 +2586,1208 @@
       <c r="J1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
-        <v>113</v>
-      </c>
-      <c r="B2">
+        <v>114</v>
+      </c>
+      <c r="B2" s="1">
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="1">
+        <v>22102</v>
+      </c>
+      <c r="H2" t="s">
+        <v>119</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="1">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G3" s="1">
+        <v>22103</v>
+      </c>
+      <c r="H3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F4" t="s">
+        <v>118</v>
+      </c>
+      <c r="G4" s="1">
+        <v>22104</v>
+      </c>
+      <c r="H4" t="s">
+        <v>130</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" t="s">
         <v>114</v>
       </c>
+      <c r="B5" s="1">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="1">
+        <v>22105</v>
+      </c>
+      <c r="H5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B6" s="1">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" t="s">
+        <v>118</v>
+      </c>
+      <c r="G6" s="1">
+        <v>22106</v>
+      </c>
+      <c r="H6" t="s">
+        <v>126</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="1">
+        <v>22107</v>
+      </c>
+      <c r="H7" t="s">
+        <v>130</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="1">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>134</v>
+      </c>
+      <c r="E8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="1">
+        <v>22108</v>
+      </c>
+      <c r="H8" t="s">
+        <v>119</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="1">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" t="s">
+        <v>118</v>
+      </c>
+      <c r="G9" s="1">
+        <v>22109</v>
+      </c>
+      <c r="H9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K9" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" s="1">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" t="s">
+        <v>136</v>
+      </c>
+      <c r="E10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" s="1">
+        <v>22110</v>
+      </c>
+      <c r="H10" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="1">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" t="s">
+        <v>137</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G11" s="1">
+        <v>22111</v>
+      </c>
+      <c r="H11" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B12" s="1">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" t="s">
+        <v>118</v>
+      </c>
+      <c r="G12" s="1">
+        <v>22112</v>
+      </c>
+      <c r="H12" t="s">
+        <v>126</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="1">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" t="s">
+        <v>139</v>
+      </c>
+      <c r="E13" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="1">
+        <v>22113</v>
+      </c>
+      <c r="H13" t="s">
+        <v>130</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B14" s="1">
+        <v>17</v>
+      </c>
+      <c r="C14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D14" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" t="s">
+        <v>117</v>
+      </c>
+      <c r="F14" t="s">
+        <v>118</v>
+      </c>
+      <c r="G14" s="1">
+        <v>22114</v>
+      </c>
+      <c r="H14" t="s">
+        <v>119</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K14" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" t="s">
+        <v>123</v>
+      </c>
+      <c r="B15" s="1">
+        <v>18</v>
+      </c>
+      <c r="C15" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" t="s">
+        <v>141</v>
+      </c>
+      <c r="E15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G15" s="1">
+        <v>22115</v>
+      </c>
+      <c r="H15" t="s">
+        <v>126</v>
+      </c>
+      <c r="I15" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" t="s">
+        <v>127</v>
+      </c>
+      <c r="B16" s="1">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" t="s">
+        <v>142</v>
+      </c>
+      <c r="E16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" t="s">
+        <v>118</v>
+      </c>
+      <c r="G16" s="1">
+        <v>22116</v>
+      </c>
+      <c r="H16" t="s">
+        <v>130</v>
+      </c>
+      <c r="I16" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="1">
+        <v>20</v>
+      </c>
+      <c r="C17" t="s">
+        <v>115</v>
+      </c>
+      <c r="D17" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="1">
+        <v>22117</v>
+      </c>
+      <c r="H17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I17" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K17" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" t="s">
+        <v>123</v>
+      </c>
+      <c r="B18" s="1">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D18" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
+        <v>118</v>
+      </c>
+      <c r="G18" s="1">
+        <v>22118</v>
+      </c>
+      <c r="H18" t="s">
+        <v>126</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B19" s="1">
+        <v>22</v>
+      </c>
+      <c r="C19" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" t="s">
+        <v>145</v>
+      </c>
+      <c r="E19" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="1">
+        <v>22119</v>
+      </c>
+      <c r="H19" t="s">
+        <v>130</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K19" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" s="1">
+        <v>23</v>
+      </c>
+      <c r="C20" t="s">
+        <v>115</v>
+      </c>
+      <c r="D20" t="s">
+        <v>146</v>
+      </c>
+      <c r="E20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="1">
+        <v>22120</v>
+      </c>
+      <c r="H20" t="s">
+        <v>119</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" t="s">
+        <v>123</v>
+      </c>
+      <c r="B21" s="1">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>124</v>
+      </c>
+      <c r="D21" t="s">
+        <v>147</v>
+      </c>
+      <c r="E21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="1">
+        <v>22121</v>
+      </c>
+      <c r="H21" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" s="1">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>128</v>
+      </c>
+      <c r="D22" t="s">
+        <v>148</v>
+      </c>
+      <c r="E22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" t="s">
+        <v>118</v>
+      </c>
+      <c r="G22" s="1">
+        <v>22122</v>
+      </c>
+      <c r="H22" t="s">
+        <v>130</v>
+      </c>
+      <c r="I22" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K22" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.94117647058824" defaultRowHeight="16.8"/>
+  <cols>
+    <col min="1" max="1" width="5.70588235294118" customWidth="1"/>
+    <col min="2" max="2" width="6.52941176470588" customWidth="1"/>
+    <col min="3" max="3" width="11.5294117647059" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="4.35294117647059" customWidth="1"/>
+    <col min="6" max="6" width="6.29411764705882" customWidth="1"/>
+    <col min="7" max="7" width="5.41176470588235" customWidth="1"/>
+    <col min="8" max="8" width="7.52941176470588" customWidth="1"/>
+    <col min="9" max="9" width="9.05882352941176" customWidth="1"/>
+    <col min="10" max="10" width="10.4705882352941" customWidth="1"/>
+    <col min="11" max="11" width="13.1764705882353" customWidth="1"/>
+    <col min="12" max="12" width="7.41176470588235" customWidth="1"/>
+    <col min="13" max="13" width="10.8235294117647" customWidth="1"/>
+    <col min="14" max="14" width="11.5294117647059"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D1" t="s">
+        <v>152</v>
+      </c>
+      <c r="E1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" t="s">
+        <v>156</v>
+      </c>
+      <c r="I1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J1" t="s">
+        <v>158</v>
+      </c>
+      <c r="K1" t="s">
+        <v>159</v>
+      </c>
+      <c r="L1" t="s">
+        <v>160</v>
+      </c>
+      <c r="M1" t="s">
+        <v>161</v>
+      </c>
+      <c r="N1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" t="s">
+        <v>165</v>
+      </c>
       <c r="D2" t="s">
-        <v>115</v>
-      </c>
-      <c r="E2" t="s">
-        <v>116</v>
+        <v>166</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>167</v>
       </c>
       <c r="G2">
-        <v>22102</v>
+        <v>2000</v>
       </c>
       <c r="H2" t="s">
-        <v>118</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J2" s="1">
-        <v>45196</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>168</v>
+      </c>
+      <c r="I2">
+        <v>123</v>
+      </c>
+      <c r="J2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" t="s">
+        <v>170</v>
+      </c>
+      <c r="L2" t="s">
+        <v>171</v>
+      </c>
+      <c r="M2">
+        <v>37067</v>
+      </c>
+      <c r="N2">
+        <v>1237151273</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3">
-        <v>6</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="B3"/>
       <c r="C3" t="s">
-        <v>121</v>
+        <v>173</v>
       </c>
       <c r="D3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E3" t="s">
-        <v>116</v>
+        <v>174</v>
+      </c>
+      <c r="E3">
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>117</v>
+        <v>175</v>
       </c>
       <c r="G3">
-        <v>22103</v>
+        <v>2001</v>
       </c>
       <c r="H3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J3" s="1">
-        <v>45197</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>176</v>
+      </c>
+      <c r="I3">
+        <v>124</v>
+      </c>
+      <c r="J3" t="s">
+        <v>177</v>
+      </c>
+      <c r="K3" t="s">
+        <v>170</v>
+      </c>
+      <c r="L3" t="s">
+        <v>171</v>
+      </c>
+      <c r="M3">
+        <v>37068</v>
+      </c>
+      <c r="N3">
+        <v>1237151274</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B4">
-        <v>7</v>
+        <v>178</v>
+      </c>
+      <c r="B4" t="s">
+        <v>179</v>
       </c>
       <c r="C4" t="s">
+        <v>180</v>
+      </c>
+      <c r="D4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E4">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4">
+        <v>2002</v>
+      </c>
+      <c r="H4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4">
         <v>125</v>
       </c>
-      <c r="D4" t="s">
+      <c r="J4" t="s">
+        <v>183</v>
+      </c>
+      <c r="K4" t="s">
+        <v>170</v>
+      </c>
+      <c r="L4" t="s">
+        <v>171</v>
+      </c>
+      <c r="M4">
+        <v>37069</v>
+      </c>
+      <c r="N4">
+        <v>1237151275</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G5">
+        <v>2003</v>
+      </c>
+      <c r="H5" t="s">
+        <v>185</v>
+      </c>
+      <c r="I5">
         <v>126</v>
       </c>
-      <c r="E4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F4" t="s">
-        <v>117</v>
-      </c>
-      <c r="G4">
-        <v>22104</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="J5" t="s">
+        <v>169</v>
+      </c>
+      <c r="K5" t="s">
+        <v>170</v>
+      </c>
+      <c r="L5" t="s">
+        <v>171</v>
+      </c>
+      <c r="M5">
+        <v>37070</v>
+      </c>
+      <c r="N5">
+        <v>1237151276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E6">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>186</v>
+      </c>
+      <c r="G6">
+        <v>2004</v>
+      </c>
+      <c r="H6" t="s">
+        <v>187</v>
+      </c>
+      <c r="I6">
         <v>127</v>
       </c>
-      <c r="I4" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J4" s="1">
-        <v>45198</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="J6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K6" t="s">
+        <v>170</v>
+      </c>
+      <c r="L6" t="s">
+        <v>171</v>
+      </c>
+      <c r="M6">
+        <v>37071</v>
+      </c>
+      <c r="N6">
+        <v>1237151277</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" t="s">
+        <v>166</v>
+      </c>
+      <c r="E7">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G7">
+        <v>2005</v>
+      </c>
+      <c r="H7" t="s">
+        <v>189</v>
+      </c>
+      <c r="I7">
         <v>128</v>
       </c>
-      <c r="E5" t="s">
-        <v>116</v>
-      </c>
-      <c r="F5" t="s">
-        <v>117</v>
-      </c>
-      <c r="G5">
-        <v>22105</v>
-      </c>
-      <c r="H5" t="s">
-        <v>118</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J5" s="1">
-        <v>45199</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="J7" t="s">
+        <v>183</v>
+      </c>
+      <c r="K7" t="s">
+        <v>170</v>
+      </c>
+      <c r="L7" t="s">
+        <v>171</v>
+      </c>
+      <c r="M7">
+        <v>37072</v>
+      </c>
+      <c r="N7">
+        <v>1237151278</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" t="s">
+        <v>165</v>
+      </c>
+      <c r="D8" t="s">
+        <v>166</v>
+      </c>
+      <c r="E8">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>190</v>
+      </c>
+      <c r="G8">
+        <v>2006</v>
+      </c>
+      <c r="H8" t="s">
+        <v>191</v>
+      </c>
+      <c r="I8">
         <v>129</v>
       </c>
-      <c r="E6" t="s">
-        <v>116</v>
-      </c>
-      <c r="F6" t="s">
-        <v>117</v>
-      </c>
-      <c r="G6">
-        <v>22106</v>
-      </c>
-      <c r="H6" t="s">
-        <v>123</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J6" s="1">
-        <v>45200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>125</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="J8" t="s">
+        <v>169</v>
+      </c>
+      <c r="K8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L8" t="s">
+        <v>171</v>
+      </c>
+      <c r="M8">
+        <v>37073</v>
+      </c>
+      <c r="N8">
+        <v>1237151279</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9">
+        <v>2007</v>
+      </c>
+      <c r="H9" t="s">
+        <v>193</v>
+      </c>
+      <c r="I9">
         <v>130</v>
       </c>
-      <c r="E7" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7">
-        <v>22107</v>
-      </c>
-      <c r="H7" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J7" s="1">
-        <v>45201</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>114</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="J9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K9" t="s">
+        <v>170</v>
+      </c>
+      <c r="L9" t="s">
+        <v>171</v>
+      </c>
+      <c r="M9">
+        <v>37074</v>
+      </c>
+      <c r="N9">
+        <v>1237151280</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" t="s">
+        <v>179</v>
+      </c>
+      <c r="C10" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" t="s">
+        <v>166</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>194</v>
+      </c>
+      <c r="G10">
+        <v>2008</v>
+      </c>
+      <c r="H10" t="s">
+        <v>195</v>
+      </c>
+      <c r="I10">
         <v>131</v>
       </c>
-      <c r="E8" t="s">
-        <v>116</v>
-      </c>
-      <c r="F8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G8">
-        <v>22108</v>
-      </c>
-      <c r="H8" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J8" s="1">
-        <v>45202</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>120</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F9" t="s">
-        <v>117</v>
-      </c>
-      <c r="G9">
-        <v>22109</v>
-      </c>
-      <c r="H9" t="s">
-        <v>123</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J9" s="1">
-        <v>45203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10">
-        <v>13</v>
-      </c>
-      <c r="C10" t="s">
-        <v>125</v>
-      </c>
-      <c r="D10" t="s">
-        <v>133</v>
-      </c>
-      <c r="E10" t="s">
-        <v>116</v>
-      </c>
-      <c r="F10" t="s">
-        <v>117</v>
-      </c>
-      <c r="G10">
-        <v>22110</v>
-      </c>
-      <c r="H10" t="s">
-        <v>127</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J10" s="1">
-        <v>45204</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B11">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>114</v>
-      </c>
-      <c r="D11" t="s">
-        <v>134</v>
-      </c>
-      <c r="E11" t="s">
-        <v>116</v>
-      </c>
-      <c r="F11" t="s">
-        <v>117</v>
-      </c>
-      <c r="G11">
-        <v>22111</v>
-      </c>
-      <c r="H11" t="s">
-        <v>118</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J11" s="1">
-        <v>45205</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B12">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>121</v>
-      </c>
-      <c r="D12" t="s">
-        <v>135</v>
-      </c>
-      <c r="E12" t="s">
-        <v>116</v>
-      </c>
-      <c r="F12" t="s">
-        <v>117</v>
-      </c>
-      <c r="G12">
-        <v>22112</v>
-      </c>
-      <c r="H12" t="s">
-        <v>123</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J12" s="1">
-        <v>45206</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B13">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>125</v>
-      </c>
-      <c r="D13" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" t="s">
-        <v>116</v>
-      </c>
-      <c r="F13" t="s">
-        <v>117</v>
-      </c>
-      <c r="G13">
-        <v>22113</v>
-      </c>
-      <c r="H13" t="s">
-        <v>127</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J13" s="1">
-        <v>45207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B14">
-        <v>17</v>
-      </c>
-      <c r="C14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" t="s">
-        <v>137</v>
-      </c>
-      <c r="E14" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" t="s">
-        <v>117</v>
-      </c>
-      <c r="G14">
-        <v>22114</v>
-      </c>
-      <c r="H14" t="s">
-        <v>118</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J14" s="1">
-        <v>45208</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15">
-        <v>18</v>
-      </c>
-      <c r="C15" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" t="s">
-        <v>138</v>
-      </c>
-      <c r="E15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F15" t="s">
-        <v>117</v>
-      </c>
-      <c r="G15">
-        <v>22115</v>
-      </c>
-      <c r="H15" t="s">
-        <v>123</v>
-      </c>
-      <c r="I15" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J15" s="1">
-        <v>45209</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>124</v>
-      </c>
-      <c r="B16">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>125</v>
-      </c>
-      <c r="D16" t="s">
-        <v>139</v>
-      </c>
-      <c r="E16" t="s">
-        <v>116</v>
-      </c>
-      <c r="F16" t="s">
-        <v>117</v>
-      </c>
-      <c r="G16">
-        <v>22116</v>
-      </c>
-      <c r="H16" t="s">
-        <v>127</v>
-      </c>
-      <c r="I16" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J16" s="1">
-        <v>45210</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10">
-      <c r="A17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B17">
-        <v>20</v>
-      </c>
-      <c r="C17" t="s">
-        <v>114</v>
-      </c>
-      <c r="D17" t="s">
-        <v>140</v>
-      </c>
-      <c r="E17" t="s">
-        <v>116</v>
-      </c>
-      <c r="F17" t="s">
-        <v>117</v>
-      </c>
-      <c r="G17">
-        <v>22117</v>
-      </c>
-      <c r="H17" t="s">
-        <v>118</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J17" s="1">
-        <v>45211</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10">
-      <c r="A18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" t="s">
-        <v>141</v>
-      </c>
-      <c r="E18" t="s">
-        <v>116</v>
-      </c>
-      <c r="F18" t="s">
-        <v>117</v>
-      </c>
-      <c r="G18">
-        <v>22118</v>
-      </c>
-      <c r="H18" t="s">
-        <v>123</v>
-      </c>
-      <c r="I18" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J18" s="1">
-        <v>45212</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>125</v>
-      </c>
-      <c r="D19" t="s">
-        <v>142</v>
-      </c>
-      <c r="E19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F19" t="s">
-        <v>117</v>
-      </c>
-      <c r="G19">
-        <v>22119</v>
-      </c>
-      <c r="H19" t="s">
-        <v>127</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J19" s="1">
-        <v>45213</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10">
-      <c r="A20" t="s">
-        <v>113</v>
-      </c>
-      <c r="B20">
-        <v>23</v>
-      </c>
-      <c r="C20" t="s">
-        <v>114</v>
-      </c>
-      <c r="D20" t="s">
-        <v>143</v>
-      </c>
-      <c r="E20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20">
-        <v>22120</v>
-      </c>
-      <c r="H20" t="s">
-        <v>118</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J20" s="1">
-        <v>45214</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10">
-      <c r="A21" t="s">
-        <v>120</v>
-      </c>
-      <c r="B21">
-        <v>24</v>
-      </c>
-      <c r="C21" t="s">
-        <v>121</v>
-      </c>
-      <c r="D21" t="s">
-        <v>144</v>
-      </c>
-      <c r="E21" t="s">
-        <v>116</v>
-      </c>
-      <c r="F21" t="s">
-        <v>117</v>
-      </c>
-      <c r="G21">
-        <v>22121</v>
-      </c>
-      <c r="H21" t="s">
-        <v>123</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J21" s="1">
-        <v>45215</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10">
-      <c r="A22" t="s">
-        <v>124</v>
-      </c>
-      <c r="B22">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>125</v>
-      </c>
-      <c r="D22" t="s">
-        <v>145</v>
-      </c>
-      <c r="E22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" t="s">
-        <v>117</v>
-      </c>
-      <c r="G22">
-        <v>22122</v>
-      </c>
-      <c r="H22" t="s">
-        <v>127</v>
-      </c>
-      <c r="I22" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="J22" s="1">
-        <v>45216</v>
+      <c r="J10" t="s">
+        <v>183</v>
+      </c>
+      <c r="K10" t="s">
+        <v>170</v>
+      </c>
+      <c r="L10" t="s">
+        <v>171</v>
+      </c>
+      <c r="M10">
+        <v>37075</v>
+      </c>
+      <c r="N10">
+        <v>1237151281</v>
       </c>
     </row>
   </sheetData>

</xml_diff>